<commit_message>
Fix Parent column title
</commit_message>
<xml_diff>
--- a/modules/core/test/com/borets/pfa/report/equip/Equipment_Utilization_Report_Template_1_2.xlsx
+++ b/modules/core/test/com/borets/pfa/report/equip/Equipment_Utilization_Report_Template_1_2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\pfa\modules\core\test\com\borets\pfa\report\equip\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,9 +26,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
-    <t>Reference code</t>
-  </si>
-  <si>
     <t>Customer</t>
   </si>
   <si>
@@ -81,6 +78,9 @@
   </si>
   <si>
     <t>{textWithBoldBorderValue}</t>
+  </si>
+  <si>
+    <t>Parent</t>
   </si>
 </sst>
 </file>
@@ -644,64 +644,64 @@
       <c r="A1" s="9"/>
       <c r="B1" s="9"/>
       <c r="C1" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="6" t="s">
-        <v>15</v>
-      </c>
       <c r="H1" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K1" s="4"/>
     </row>
     <row r="2" spans="1:11" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="3" t="s">
-        <v>8</v>
-      </c>
       <c r="K2" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add equipment-type column to report
</commit_message>
<xml_diff>
--- a/modules/core/test/com/borets/pfa/report/equip/Equipment_Utilization_Report_Template_1_2.xlsx
+++ b/modules/core/test/com/borets/pfa/report/equip/Equipment_Utilization_Report_Template_1_2.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Customer</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>Parent</t>
+  </si>
+  <si>
+    <t>Equipment Type</t>
   </si>
 </sst>
 </file>
@@ -619,11 +622,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:B1"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -631,16 +634,16 @@
     <col min="1" max="1" width="20" customWidth="1"/>
     <col min="2" max="2" width="17.85546875" customWidth="1"/>
     <col min="3" max="3" width="18.140625" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" customWidth="1"/>
-    <col min="6" max="6" width="30.7109375" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" customWidth="1"/>
-    <col min="9" max="10" width="9.7109375" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" customWidth="1"/>
+    <col min="4" max="5" width="12.42578125" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" customWidth="1"/>
+    <col min="7" max="7" width="30.7109375" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" customWidth="1"/>
+    <col min="10" max="11" width="9.7109375" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9"/>
       <c r="B1" s="9"/>
       <c r="C1" s="8" t="s">
@@ -649,27 +652,28 @@
       <c r="D1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="7"/>
+      <c r="F1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
     </row>
-    <row r="2" spans="1:11" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>18</v>
       </c>
@@ -683,28 +687,31 @@
         <v>1</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -716,6 +723,7 @@
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>